<commit_message>
Stand up weeks 8, 9 y 10
</commit_message>
<xml_diff>
--- a/Semana 12-16 octubre/Stand_Up_Meeitng_Week_8.xlsx
+++ b/Semana 12-16 octubre/Stand_Up_Meeitng_Week_8.xlsx
@@ -5,35 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\GitHub\Ingenieria_Software\Semana 12-16 octubre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula\Documents\GitHub\Ingenieria_Software\Semana 12-16 octubre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84DEC3DE-2C46-4B86-B982-C5E6FE92228E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A61466-4626-4785-9CC7-798230E6DEB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t xml:space="preserve"> MIEMBRO</t>
   </si>
@@ -104,6 +96,42 @@
   </si>
   <si>
     <t>SEMANA 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nada </t>
+  </si>
+  <si>
+    <t>Problemas personales</t>
+  </si>
+  <si>
+    <t>Nada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No hubo clase </t>
+  </si>
+  <si>
+    <t>Planeamos reunión para mañana</t>
+  </si>
+  <si>
+    <t>Otras materias</t>
+  </si>
+  <si>
+    <t>Ordenar la reunión de hoy</t>
+  </si>
+  <si>
+    <t>Ninguna</t>
+  </si>
+  <si>
+    <t>Reunión para revisar y opinar el trabajo de Mariana</t>
+  </si>
+  <si>
+    <t>Reunirnos, revisar diagramas y Mariana comenzará con las tablas</t>
+  </si>
+  <si>
+    <t>Parcial mañana</t>
+  </si>
+  <si>
+    <t>Se logró el objetivo y se encontró el diagrama que faltaba</t>
   </si>
 </sst>
 </file>
@@ -720,28 +748,28 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.453125" customWidth="1"/>
-    <col min="2" max="2" width="24.36328125" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="26.36328125" customWidth="1"/>
-    <col min="5" max="5" width="23.36328125" customWidth="1"/>
-    <col min="6" max="6" width="23.08984375" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" customWidth="1"/>
-    <col min="11" max="11" width="4.6328125" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" customWidth="1"/>
+    <col min="11" max="11" width="4.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.21875" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="10.26953125" customWidth="1"/>
+    <col min="14" max="14" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>15</v>
       </c>
@@ -759,7 +787,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -775,7 +803,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -798,7 +826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>10</v>
       </c>
@@ -811,7 +839,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="12" t="s">
         <v>8</v>
@@ -822,7 +850,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16"/>
       <c r="B6" s="3" t="s">
         <v>9</v>
@@ -833,7 +861,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
@@ -846,7 +874,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="12" t="s">
         <v>8</v>
@@ -857,7 +885,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="16"/>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -868,42 +896,72 @@
       <c r="F9" s="7"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
       <c r="B11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16"/>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>13</v>
       </c>
@@ -916,7 +974,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="12" t="s">
         <v>8</v>
@@ -927,7 +985,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
@@ -938,7 +996,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>14</v>
       </c>
@@ -951,7 +1009,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="15"/>
       <c r="B17" s="12" t="s">
         <v>8</v>
@@ -962,7 +1020,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16"/>
       <c r="B18" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Stand Ups AcTuAlIzAdOs aAaAaA siempre se me olvida
</commit_message>
<xml_diff>
--- a/Semana 12-16 octubre/Stand_Up_Meeitng_Week_8.xlsx
+++ b/Semana 12-16 octubre/Stand_Up_Meeitng_Week_8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula\Documents\GitHub\Ingenieria_Software\Semana 12-16 octubre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\GitHub\Ingenieria_Software\Semana 12-16 octubre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A61466-4626-4785-9CC7-798230E6DEB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3543B360-1A5A-4DD2-A04E-17E8983941DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
+    <workbookView xWindow="708" yWindow="2208" windowWidth="21348" windowHeight="8100" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t xml:space="preserve"> MIEMBRO</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Se logró el objetivo y se encontró el diagrama que faltaba</t>
+  </si>
+  <si>
+    <t>Planeación de reunión</t>
   </si>
 </sst>
 </file>
@@ -747,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4E8726-24EF-4B21-B937-D55FA5E6EA95}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1003,33 +1006,63 @@
       <c r="B16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="15"/>
       <c r="B17" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16"/>
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>